<commit_message>
acrescido nome do projeto na plinha de cobertura
</commit_message>
<xml_diff>
--- a/cobertura.xlsx
+++ b/cobertura.xlsx
@@ -67,15 +67,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.58988764044944"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="52.58988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.589887640449438"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.58988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="52.58988764044944"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.88988764044944"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -98,1440 +99,1920 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
           <t>AuthenticationInfoAWSCredentialsProvider</t>
         </is>
       </c>
-      <c r="B2" s="0" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>AuthenticationInfoAWSCredentialsProvider(AuthenticationInfo)</t>
         </is>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
           <t>AuthenticationInfoAWSCredentialsProvider</t>
         </is>
       </c>
-      <c r="B3" s="0" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>getCredentials() : AWSCredentials</t>
         </is>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
           <t>AuthenticationInfoAWSCredentialsProvider</t>
         </is>
       </c>
-      <c r="B4" s="0" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>refresh() : void</t>
         </is>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
           <t>AuthenticationInfoAWSCredentialsProviderChain</t>
         </is>
       </c>
-      <c r="B5" s="0" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>AuthenticationInfoAWSCredentialsProviderChain(AuthenticationInfo)</t>
         </is>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="D5" s="0" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
           <t>AuthenticationInfoAWSCredentials</t>
         </is>
       </c>
-      <c r="B6" s="0" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>AuthenticationInfoAWSCredentials(AuthenticationInfo)</t>
         </is>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="D6" s="0" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
           <t>AuthenticationInfoAWSCredentials</t>
         </is>
       </c>
-      <c r="B7" s="0" t="inlineStr">
+      <c r="C7" s="0" t="inlineStr">
         <is>
           <t>getAWSAccessKeyId() : String</t>
         </is>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="D7" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
           <t>AuthenticationInfoAWSCredentials</t>
         </is>
       </c>
-      <c r="B8" s="0" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>getAWSSecretKey() : String</t>
         </is>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="D8" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B9" s="0" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>SimpleStorageServiceWagon()</t>
         </is>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="D9" s="0" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B10" s="0" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>SimpleStorageServiceWagon(AmazonS3,String,String)</t>
         </is>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="D10" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B11" s="0" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>connectToRepository(Repository,AuthenticationInfo,ProxyInfoProvider) : void</t>
         </is>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="D11" s="0" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B12" s="0" t="inlineStr">
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>disconnectFromRepository() : void</t>
         </is>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="D12" s="0" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B13" s="0" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>doesRemoteResourceExist(String) : boolean</t>
         </is>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="D13" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B14" s="0" t="inlineStr">
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>isRemoteResourceNewer(String,long) : boolean</t>
         </is>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="D14" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B15" s="0" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>listDirectory(String) : List&lt;String&gt;</t>
         </is>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="D15" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B16" s="0" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>getResource(String,File,TransferProgress) : void</t>
         </is>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="D16" s="0" t="n">
         <v>0.8181818</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B17" s="0" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>putResource(File,String,TransferProgress) : void</t>
         </is>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="D17" s="0" t="n">
         <v>0.9166667</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B18" s="0" t="inlineStr">
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>getObjectMetadata(String) : ObjectMetadata</t>
         </is>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="D18" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B19" s="0" t="inlineStr">
+      <c r="C19" s="0" t="inlineStr">
         <is>
           <t>getKey(String) : String</t>
         </is>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="D19" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B20" s="0" t="inlineStr">
+      <c r="C20" s="0" t="inlineStr">
         <is>
           <t>getResourceNames(ObjectListing,Pattern) : List&lt;String&gt;</t>
         </is>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="D20" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B21" s="0" t="inlineStr">
+      <c r="C21" s="0" t="inlineStr">
         <is>
           <t>getResourceName(String,Pattern) : String</t>
         </is>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="D21" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B22" s="0" t="inlineStr">
+      <c r="C22" s="0" t="inlineStr">
         <is>
           <t>mkdirs(String,int) : void</t>
         </is>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="D22" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
           <t>SimpleStorageServiceWagon</t>
         </is>
       </c>
-      <c r="B23" s="0" t="inlineStr">
+      <c r="C23" s="0" t="inlineStr">
         <is>
           <t>createDirectoryPutObjectRequest(String) : PutObjectRequest</t>
         </is>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="D23" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
           <t>IoUtils</t>
         </is>
       </c>
-      <c r="B24" s="0" t="inlineStr">
+      <c r="C24" s="0" t="inlineStr">
         <is>
           <t>IoUtils()</t>
         </is>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="D24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
           <t>IoUtils</t>
         </is>
       </c>
-      <c r="B25" s="0" t="inlineStr">
+      <c r="C25" s="0" t="inlineStr">
         <is>
           <t>copy(InputStream,OutputStream) : void</t>
         </is>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="D25" s="0" t="n">
         <v>0.75</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B26" s="0" t="inlineStr">
+        <is>
           <t>IoUtils</t>
         </is>
       </c>
-      <c r="B26" s="0" t="inlineStr">
+      <c r="C26" s="0" t="inlineStr">
         <is>
           <t>closeQuietly(Closeable) : void</t>
         </is>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="D26" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B27" s="0" t="inlineStr">
+        <is>
           <t>S3Utils</t>
         </is>
       </c>
-      <c r="B27" s="0" t="inlineStr">
+      <c r="C27" s="0" t="inlineStr">
         <is>
           <t>S3Utils()</t>
         </is>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="D27" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B28" s="0" t="inlineStr">
+        <is>
           <t>S3Utils</t>
         </is>
       </c>
-      <c r="B28" s="0" t="inlineStr">
+      <c r="C28" s="0" t="inlineStr">
         <is>
           <t>getBucketName(Repository) : String</t>
         </is>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="D28" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B29" s="0" t="inlineStr">
+        <is>
           <t>S3Utils</t>
         </is>
       </c>
-      <c r="B29" s="0" t="inlineStr">
+      <c r="C29" s="0" t="inlineStr">
         <is>
           <t>getBaseDirectory(Repository) : String</t>
         </is>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="D29" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B30" s="0" t="inlineStr">
+        <is>
           <t>S3Utils</t>
         </is>
       </c>
-      <c r="B30" s="0" t="inlineStr">
+      <c r="C30" s="0" t="inlineStr">
         <is>
           <t>getClientConfiguration(ProxyInfoProvider) : ClientConfiguration</t>
         </is>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="D30" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C31" s="0" t="inlineStr">
+        <is>
           <t>AbstractWagon(boolean)</t>
         </is>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="D31" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="inlineStr">
+        <is>
           <t>AbstractWagon(boolean,SessionListenerSupport,TransferListenerSupport)</t>
         </is>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="D32" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="inlineStr">
+        <is>
           <t>addSessionListener(SessionListener) : void</t>
         </is>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="D33" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="inlineStr">
+        <is>
           <t>hasSessionListener(SessionListener) : boolean</t>
         </is>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="D34" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="inlineStr">
+        <is>
           <t>removeSessionListener(SessionListener) : void</t>
         </is>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="D35" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="inlineStr">
+        <is>
           <t>addTransferListener(TransferListener) : void</t>
         </is>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="D36" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="inlineStr">
+        <is>
           <t>hasTransferListener(TransferListener) : boolean</t>
         </is>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="D37" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="inlineStr">
+        <is>
           <t>removeTransferListener(TransferListener) : void</t>
         </is>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="D38" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B39" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="inlineStr">
+        <is>
           <t>getRepository() : Repository</t>
         </is>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="D39" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B40" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="inlineStr">
+        <is>
           <t>isInteractive() : boolean</t>
         </is>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="D40" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B41" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
           <t>setInteractive(boolean) : void</t>
         </is>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="D41" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B42" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="inlineStr">
+        <is>
           <t>connect(Repository) : void</t>
         </is>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="D42" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B43" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="inlineStr">
+        <is>
           <t>connect(Repository,ProxyInfo) : void</t>
         </is>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="D43" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B44" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="inlineStr">
+        <is>
           <t>connect(Repository,AuthenticationInfo) : void</t>
         </is>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="D44" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="inlineStr">
+        <is>
           <t>connect(Repository,ProxyInfoProvider) : void</t>
         </is>
       </c>
-      <c r="C45" s="0" t="n">
+      <c r="D45" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B46" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
           <t>connect(Repository,AuthenticationInfo,ProxyInfo) : void</t>
         </is>
       </c>
-      <c r="C46" s="0" t="n">
+      <c r="D46" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="inlineStr">
+        <is>
           <t>connect(Repository,AuthenticationInfo,ProxyInfoProvider) : void</t>
         </is>
       </c>
-      <c r="C47" s="0" t="n">
+      <c r="D47" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="inlineStr">
+        <is>
           <t>disconnect() : void</t>
         </is>
       </c>
-      <c r="C48" s="0" t="n">
+      <c r="D48" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="inlineStr">
+        <is>
           <t>get(String,File) : void</t>
         </is>
       </c>
-      <c r="C49" s="0" t="n">
+      <c r="D49" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B50" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="inlineStr">
+        <is>
           <t>getFileList(String) : List&lt;String&gt;</t>
         </is>
       </c>
-      <c r="C50" s="0" t="n">
+      <c r="D50" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B51" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="inlineStr">
+        <is>
           <t>getIfNewer(String,File,long) : boolean</t>
         </is>
       </c>
-      <c r="C51" s="0" t="n">
+      <c r="D51" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B52" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C52" s="0" t="inlineStr">
+        <is>
           <t>openConnection() : void</t>
         </is>
       </c>
-      <c r="C52" s="0" t="n">
+      <c r="D52" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B53" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C53" s="0" t="inlineStr">
+        <is>
           <t>put(File,String) : void</t>
         </is>
       </c>
-      <c r="C53" s="0" t="n">
+      <c r="D53" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B54" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C54" s="0" t="inlineStr">
+        <is>
           <t>putDirectory(File,String) : void</t>
         </is>
       </c>
-      <c r="C54" s="0" t="n">
+      <c r="D54" s="0" t="n">
         <v>0.8333333</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B55" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C55" s="0" t="inlineStr">
+        <is>
           <t>resourceExists(String) : boolean</t>
         </is>
       </c>
-      <c r="C55" s="0" t="n">
+      <c r="D55" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B56" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C56" s="0" t="inlineStr">
+        <is>
           <t>supportsDirectoryCopy() : boolean</t>
         </is>
       </c>
-      <c r="C56" s="0" t="n">
+      <c r="D56" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B57" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C57" s="0" t="inlineStr">
+        <is>
           <t>getReadTimeout() : int</t>
         </is>
       </c>
-      <c r="C57" s="0" t="n">
+      <c r="D57" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B58" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C58" s="0" t="inlineStr">
+        <is>
           <t>setReadTimeout(int) : void</t>
         </is>
       </c>
-      <c r="C58" s="0" t="n">
+      <c r="D58" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B59" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C59" s="0" t="inlineStr">
+        <is>
           <t>getTimeout() : int</t>
         </is>
       </c>
-      <c r="C59" s="0" t="n">
+      <c r="D59" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>AbstractWagon</t>
+          <t>aws-maven</t>
         </is>
       </c>
       <c r="B60" s="0" t="inlineStr">
         <is>
+          <t>AbstractWagon</t>
+        </is>
+      </c>
+      <c r="C60" s="0" t="inlineStr">
+        <is>
           <t>setTimeout(int) : void</t>
         </is>
       </c>
-      <c r="C60" s="0" t="n">
+      <c r="D60" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B61" s="0" t="inlineStr">
+        <is>
           <t>NullProtectingProxyInfoProvider</t>
         </is>
       </c>
-      <c r="B61" s="0" t="inlineStr">
+      <c r="C61" s="0" t="inlineStr">
         <is>
           <t>NullProtectingProxyInfoProvider(ProxyInfo)</t>
         </is>
       </c>
-      <c r="C61" s="0" t="n">
+      <c r="D61" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B62" s="0" t="inlineStr">
+        <is>
           <t>NullProtectingProxyInfoProvider</t>
         </is>
       </c>
-      <c r="B62" s="0" t="inlineStr">
+      <c r="C62" s="0" t="inlineStr">
         <is>
           <t>getProxyInfo(String) : ProxyInfo</t>
         </is>
       </c>
-      <c r="C62" s="0" t="n">
+      <c r="D62" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B63" s="0" t="inlineStr">
+        <is>
           <t>Region</t>
         </is>
       </c>
-      <c r="B63" s="0" t="inlineStr">
+      <c r="C63" s="0" t="inlineStr">
         <is>
           <t>Region(String,String)</t>
         </is>
       </c>
-      <c r="C63" s="0" t="n">
+      <c r="D63" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B64" s="0" t="inlineStr">
+        <is>
           <t>Region</t>
         </is>
       </c>
-      <c r="B64" s="0" t="inlineStr">
+      <c r="C64" s="0" t="inlineStr">
         <is>
           <t>getEndpoint() : String</t>
         </is>
       </c>
-      <c r="C64" s="0" t="n">
+      <c r="D64" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B65" s="0" t="inlineStr">
+        <is>
           <t>Region</t>
         </is>
       </c>
-      <c r="B65" s="0" t="inlineStr">
+      <c r="C65" s="0" t="inlineStr">
         <is>
           <t>getLocationConstraint() : String</t>
         </is>
       </c>
-      <c r="C65" s="0" t="n">
+      <c r="D65" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B66" s="0" t="inlineStr">
+        <is>
           <t>Region</t>
         </is>
       </c>
-      <c r="B66" s="0" t="inlineStr">
+      <c r="C66" s="0" t="inlineStr">
         <is>
           <t>fromLocationConstraint(String) : Region</t>
         </is>
       </c>
-      <c r="C66" s="0" t="n">
+      <c r="D66" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B67" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B67" s="0" t="inlineStr">
+      <c r="C67" s="0" t="inlineStr">
         <is>
           <t>StandardSessionListenerSupport(Wagon)</t>
         </is>
       </c>
-      <c r="C67" s="0" t="n">
+      <c r="D67" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B68" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B68" s="0" t="inlineStr">
+      <c r="C68" s="0" t="inlineStr">
         <is>
           <t>addSessionListener(SessionListener) : void</t>
         </is>
       </c>
-      <c r="C68" s="0" t="n">
+      <c r="D68" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B69" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B69" s="0" t="inlineStr">
+      <c r="C69" s="0" t="inlineStr">
         <is>
           <t>removeSessionListener(SessionListener) : void</t>
         </is>
       </c>
-      <c r="C69" s="0" t="n">
+      <c r="D69" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B70" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B70" s="0" t="inlineStr">
+      <c r="C70" s="0" t="inlineStr">
         <is>
           <t>hasSessionListener(SessionListener) : boolean</t>
         </is>
       </c>
-      <c r="C70" s="0" t="n">
+      <c r="D70" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B71" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B71" s="0" t="inlineStr">
+      <c r="C71" s="0" t="inlineStr">
         <is>
           <t>fireSessionOpening() : void</t>
         </is>
       </c>
-      <c r="C71" s="0" t="n">
+      <c r="D71" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B72" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B72" s="0" t="inlineStr">
+      <c r="C72" s="0" t="inlineStr">
         <is>
           <t>fireSessionOpened() : void</t>
         </is>
       </c>
-      <c r="C72" s="0" t="n">
+      <c r="D72" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B73" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B73" s="0" t="inlineStr">
+      <c r="C73" s="0" t="inlineStr">
         <is>
           <t>fireSessionDisconnecting() : void</t>
         </is>
       </c>
-      <c r="C73" s="0" t="n">
+      <c r="D73" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B74" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B74" s="0" t="inlineStr">
+      <c r="C74" s="0" t="inlineStr">
         <is>
           <t>fireSessionDisconnected() : void</t>
         </is>
       </c>
-      <c r="C74" s="0" t="n">
+      <c r="D74" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B75" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B75" s="0" t="inlineStr">
+      <c r="C75" s="0" t="inlineStr">
         <is>
           <t>fireSessionConnectionRefused() : void</t>
         </is>
       </c>
-      <c r="C75" s="0" t="n">
+      <c r="D75" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B76" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B76" s="0" t="inlineStr">
+      <c r="C76" s="0" t="inlineStr">
         <is>
           <t>fireSessionLoggedIn() : void</t>
         </is>
       </c>
-      <c r="C76" s="0" t="n">
+      <c r="D76" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B77" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B77" s="0" t="inlineStr">
+      <c r="C77" s="0" t="inlineStr">
         <is>
           <t>fireSessionLoggedOff() : void</t>
         </is>
       </c>
-      <c r="C77" s="0" t="n">
+      <c r="D77" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B78" s="0" t="inlineStr">
+        <is>
           <t>StandardSessionListenerSupport</t>
         </is>
       </c>
-      <c r="B78" s="0" t="inlineStr">
+      <c r="C78" s="0" t="inlineStr">
         <is>
           <t>fireSessionError(Exception) : void</t>
         </is>
       </c>
-      <c r="C78" s="0" t="n">
+      <c r="D78" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B79" s="0" t="inlineStr">
+        <is>
           <t>StandardTransferListenerSupport</t>
         </is>
       </c>
-      <c r="B79" s="0" t="inlineStr">
+      <c r="C79" s="0" t="inlineStr">
         <is>
           <t>StandardTransferListenerSupport(Wagon)</t>
         </is>
       </c>
-      <c r="C79" s="0" t="n">
+      <c r="D79" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B80" s="0" t="inlineStr">
+        <is>
           <t>StandardTransferListenerSupport</t>
         </is>
       </c>
-      <c r="B80" s="0" t="inlineStr">
+      <c r="C80" s="0" t="inlineStr">
         <is>
           <t>addTransferListener(TransferListener) : void</t>
         </is>
       </c>
-      <c r="C80" s="0" t="n">
+      <c r="D80" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B81" s="0" t="inlineStr">
+        <is>
           <t>StandardTransferListenerSupport</t>
         </is>
       </c>
-      <c r="B81" s="0" t="inlineStr">
+      <c r="C81" s="0" t="inlineStr">
         <is>
           <t>removeTransferListener(TransferListener) : void</t>
         </is>
       </c>
-      <c r="C81" s="0" t="n">
+      <c r="D81" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B82" s="0" t="inlineStr">
+        <is>
           <t>StandardTransferListenerSupport</t>
         </is>
       </c>
-      <c r="B82" s="0" t="inlineStr">
+      <c r="C82" s="0" t="inlineStr">
         <is>
           <t>hasTransferListener(TransferListener) : boolean</t>
         </is>
       </c>
-      <c r="C82" s="0" t="n">
+      <c r="D82" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B83" s="0" t="inlineStr">
+        <is>
           <t>StandardTransferListenerSupport</t>
         </is>
       </c>
-      <c r="B83" s="0" t="inlineStr">
+      <c r="C83" s="0" t="inlineStr">
         <is>
           <t>fireTransferInitiated(Resource,int) : void</t>
         </is>
       </c>
-      <c r="C83" s="0" t="n">
+      <c r="D83" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B84" s="0" t="inlineStr">
+        <is>
           <t>StandardTransferListenerSupport</t>
         </is>
       </c>
-      <c r="B84" s="0" t="inlineStr">
+      <c r="C84" s="0" t="inlineStr">
         <is>
           <t>fireTransferStarted(Resource,int) : void</t>
         </is>
       </c>
-      <c r="C84" s="0" t="n">
+      <c r="D84" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B85" s="0" t="inlineStr">
+        <is>
           <t>StandardTransferListenerSupport</t>
         </is>
       </c>
-      <c r="B85" s="0" t="inlineStr">
+      <c r="C85" s="0" t="inlineStr">
         <is>
           <t>fireTransferProgress(Resource,int,byte[],int) : void</t>
         </is>
       </c>
-      <c r="C85" s="0" t="n">
+      <c r="D85" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B86" s="0" t="inlineStr">
+        <is>
           <t>StandardTransferListenerSupport</t>
         </is>
       </c>
-      <c r="B86" s="0" t="inlineStr">
+      <c r="C86" s="0" t="inlineStr">
         <is>
           <t>fireTransferCompleted(Resource,int) : void</t>
         </is>
       </c>
-      <c r="C86" s="0" t="n">
+      <c r="D86" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B87" s="0" t="inlineStr">
+        <is>
           <t>StandardTransferListenerSupport</t>
         </is>
       </c>
-      <c r="B87" s="0" t="inlineStr">
+      <c r="C87" s="0" t="inlineStr">
         <is>
           <t>fireTransferError(Resource,int,Exception) : void</t>
         </is>
       </c>
-      <c r="C87" s="0" t="n">
+      <c r="D87" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B88" s="0" t="inlineStr">
+        <is>
           <t>StandardTransferProgress</t>
         </is>
       </c>
-      <c r="B88" s="0" t="inlineStr">
+      <c r="C88" s="0" t="inlineStr">
         <is>
           <t>StandardTransferProgress(Resource,int,TransferListenerSupport)</t>
         </is>
       </c>
-      <c r="C88" s="0" t="n">
+      <c r="D88" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B89" s="0" t="inlineStr">
+        <is>
           <t>StandardTransferProgress</t>
         </is>
       </c>
-      <c r="B89" s="0" t="inlineStr">
+      <c r="C89" s="0" t="inlineStr">
         <is>
           <t>notify(byte[],int) : void</t>
         </is>
       </c>
-      <c r="C89" s="0" t="n">
+      <c r="D89" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B90" s="0" t="inlineStr">
+        <is>
           <t>TransferProgressFileInputStream</t>
         </is>
       </c>
-      <c r="B90" s="0" t="inlineStr">
+      <c r="C90" s="0" t="inlineStr">
         <is>
           <t>TransferProgressFileInputStream(File,TransferProgress)</t>
         </is>
       </c>
-      <c r="C90" s="0" t="n">
+      <c r="D90" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B91" s="0" t="inlineStr">
+        <is>
           <t>TransferProgressFileInputStream</t>
         </is>
       </c>
-      <c r="B91" s="0" t="inlineStr">
+      <c r="C91" s="0" t="inlineStr">
         <is>
           <t>read() : int</t>
         </is>
       </c>
-      <c r="C91" s="0" t="n">
+      <c r="D91" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B92" s="0" t="inlineStr">
+        <is>
           <t>TransferProgressFileInputStream</t>
         </is>
       </c>
-      <c r="B92" s="0" t="inlineStr">
+      <c r="C92" s="0" t="inlineStr">
         <is>
           <t>read(byte[]) : int</t>
         </is>
       </c>
-      <c r="C92" s="0" t="n">
+      <c r="D92" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B93" s="0" t="inlineStr">
+        <is>
           <t>TransferProgressFileInputStream</t>
         </is>
       </c>
-      <c r="B93" s="0" t="inlineStr">
+      <c r="C93" s="0" t="inlineStr">
         <is>
           <t>read(byte[],int,int) : int</t>
         </is>
       </c>
-      <c r="C93" s="0" t="n">
+      <c r="D93" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B94" s="0" t="inlineStr">
+        <is>
           <t>TransferProgressFileOutputStream</t>
         </is>
       </c>
-      <c r="B94" s="0" t="inlineStr">
+      <c r="C94" s="0" t="inlineStr">
         <is>
           <t>TransferProgressFileOutputStream(File,TransferProgress)</t>
         </is>
       </c>
-      <c r="C94" s="0" t="n">
+      <c r="D94" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B95" s="0" t="inlineStr">
+        <is>
           <t>TransferProgressFileOutputStream</t>
         </is>
       </c>
-      <c r="B95" s="0" t="inlineStr">
+      <c r="C95" s="0" t="inlineStr">
         <is>
           <t>write(int) : void</t>
         </is>
       </c>
-      <c r="C95" s="0" t="n">
+      <c r="D95" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B96" s="0" t="inlineStr">
+        <is>
           <t>TransferProgressFileOutputStream</t>
         </is>
       </c>
-      <c r="B96" s="0" t="inlineStr">
+      <c r="C96" s="0" t="inlineStr">
         <is>
           <t>write(byte[]) : void</t>
         </is>
       </c>
-      <c r="C96" s="0" t="n">
+      <c r="D96" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
+          <t>aws-maven</t>
+        </is>
+      </c>
+      <c r="B97" s="0" t="inlineStr">
+        <is>
           <t>TransferProgressFileOutputStream</t>
         </is>
       </c>
-      <c r="B97" s="0" t="inlineStr">
+      <c r="C97" s="0" t="inlineStr">
         <is>
           <t>write(byte[],int,int) : void</t>
         </is>
       </c>
-      <c r="C97" s="0" t="n">
+      <c r="D97" s="0" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>